<commit_message>
Older results for shooter with more than 8 results no longer deleted.
</commit_message>
<xml_diff>
--- a/HaurRanking/src/test/java/haur_ranking/test/HaurRanking.xlsx
+++ b/HaurRanking/src/test/java/haur_ranking/test/HaurRanking.xlsx
@@ -529,7 +529,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
@@ -782,7 +782,7 @@
         <v>3.25</v>
       </c>
       <c r="E18" s="7">
-        <v>1.95</v>
+        <v>4.5</v>
       </c>
       <c r="F18" s="7">
         <v>5.15</v>
@@ -866,7 +866,7 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16">
-        <v>2</v>
+        <v>0.86667000000000005</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16">
@@ -883,7 +883,7 @@
         <v>0.56603999999999999</v>
       </c>
       <c r="L22" s="16">
-        <v>1.1555</v>
+        <v>0.87204000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="4">
-        <v>0.92</v>
+        <v>0.7</v>
       </c>
       <c r="L28" s="9"/>
     </row>

</xml_diff>